<commit_message>
1. finish process report script coding for ookla speedtest result
</commit_message>
<xml_diff>
--- a/throughput.xlsx
+++ b/throughput.xlsx
@@ -4,21 +4,60 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="15480" windowHeight="24600"/>
+    <workbookView windowWidth="15480" windowHeight="25020"/>
   </bookViews>
   <sheets>
-    <sheet name="DUT" sheetId="1" r:id="rId1"/>
+    <sheet name="WAN" sheetId="1" r:id="rId1"/>
     <sheet name="LAN" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="DUT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
   <si>
-    <t>DUT 2 WiFi/WiFi 2 DUT</t>
+    <t>WAN 2 WiFi/WiFi 2 WAN</t>
+  </si>
+  <si>
+    <t>CH11</t>
+  </si>
+  <si>
+    <t>CH149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downlink(Mbps)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uplink(Mbps) </t>
+  </si>
+  <si>
+    <t>Throughput on this page is generated by Ookla speedtest</t>
+  </si>
+  <si>
+    <t>PSK2</t>
+  </si>
+  <si>
+    <t>CLEAR</t>
+  </si>
+  <si>
+    <t>CH11 WRELAY</t>
+  </si>
+  <si>
+    <t>CH149 WRELAY</t>
+  </si>
+  <si>
+    <t>CH11 RELAY</t>
+  </si>
+  <si>
+    <t>CH149 RELAY</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>LAN 2 WiFi/WiFi 2 LAN</t>
   </si>
   <si>
     <t>CH36 20M</t>
@@ -27,19 +66,10 @@
     <t>CH1 20M</t>
   </si>
   <si>
-    <t xml:space="preserve">Downlink(Mbps)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uplink(Mbps) </t>
+    <t>Throughput on this page is generated by iperf2</t>
   </si>
   <si>
     <t>BREAK means iperf stream break off</t>
-  </si>
-  <si>
-    <t>PSK2</t>
-  </si>
-  <si>
-    <t>CLEAR</t>
   </si>
   <si>
     <t>ERROR means iperf running for error</t>
@@ -105,7 +135,7 @@
     <t>CH36 160M</t>
   </si>
   <si>
-    <t>LAN 2 WiFi/WiFi 2 LAN</t>
+    <t>DUT 2 WiFi/WiFi 2 DUT</t>
   </si>
 </sst>
 </file>
@@ -113,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -171,16 +201,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,14 +244,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,32 +271,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -284,6 +306,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,16 +331,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,6 +366,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -349,6 +391,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,31 +420,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +456,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,6 +492,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -450,19 +510,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,37 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,41 +560,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,6 +580,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,16 +642,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -645,133 +675,133 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -790,9 +820,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1137,20 +1167,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
-    <col min="6" max="6" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="9.125" customWidth="1"/>
-    <col min="12" max="12" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="6" max="6" width="2.875" customWidth="1"/>
+    <col min="11" max="11" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1179,7 +1206,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" ht="23.25" customHeight="1" spans="1:6">
+    <row r="3" ht="23.25" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1187,7 +1214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="2:14">
+    <row r="4" ht="15.75" spans="2:11">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1203,10 +1230,8 @@
       <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" spans="2:11">
+    </row>
+    <row r="5" ht="15.75" spans="2:10">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1230,9 +1255,6 @@
       </c>
       <c r="J5" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -1290,15 +1312,15 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" ht="23.25" customHeight="1" spans="1:6">
+    <row r="11" ht="23.25" spans="1:6">
       <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" spans="2:9">
+    </row>
+    <row r="12" ht="15.75" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="2:10">
+    <row r="13" ht="15.75" spans="2:10">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1393,15 +1415,15 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" ht="23.25" customHeight="1" spans="1:6">
+    <row r="19" ht="23.25" spans="1:6">
       <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1" spans="2:9">
+    </row>
+    <row r="20" ht="15.75" spans="2:9">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -1415,7 +1437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="2:10">
+    <row r="21" ht="15.75" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1496,29 +1518,26 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" ht="23.25" customHeight="1" spans="1:6">
+    <row r="27" ht="23.25" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" spans="2:9">
+        <v>12</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" ht="15.75" spans="2:10">
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1" spans="2:10">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" ht="15.75" spans="2:10">
       <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1531,18 +1550,11 @@
       <c r="E29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="5"/>
@@ -1588,773 +1600,54 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:5">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" ht="23.25" customHeight="1" spans="1:6">
-      <c r="A35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" spans="2:9">
-      <c r="B36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" spans="2:10">
-      <c r="B37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
+    </row>
+    <row r="35" ht="15.75" spans="2:4">
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" ht="15.75" spans="2:5">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="2:10">
+    </row>
+    <row r="39" spans="2:5">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="2:10">
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="2:10">
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="2:10">
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" ht="23.25" customHeight="1" spans="1:6">
-      <c r="A43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1" spans="2:9">
-      <c r="B44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1" spans="2:10">
-      <c r="B45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10">
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="2:10">
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="2:10">
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="2:10">
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="2:10">
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" ht="23.25" customHeight="1" spans="1:6">
-      <c r="A51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1" spans="2:9">
-      <c r="B52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1" spans="2:10">
-      <c r="B53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10">
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="2:10">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="2:10">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="2:10">
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-    </row>
-    <row r="58" spans="2:10">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" ht="23.25" customHeight="1" spans="1:6">
-      <c r="A59" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1" spans="2:9">
-      <c r="B60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1" spans="2:10">
-      <c r="B61" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10">
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="2:10">
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="2:10">
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="2:10">
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="2:10">
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A67" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B68" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B69" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5">
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="2:5">
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A75" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B76" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B77" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5">
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="2:5">
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="2:5">
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="2:5">
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="2:5">
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A83" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B84" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B85" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5">
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-    </row>
-    <row r="87" spans="2:5">
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-    </row>
-    <row r="88" spans="2:5">
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-    </row>
-    <row r="89" spans="2:5">
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-    </row>
-    <row r="90" spans="2:5">
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-    </row>
-    <row r="91" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A91" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="92" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B92" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B93" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5">
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-    </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-    </row>
-    <row r="96" spans="2:5">
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-    </row>
-    <row r="97" spans="2:5">
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-    </row>
-    <row r="98" spans="2:5">
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-    </row>
-    <row r="99" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A99" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B100" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B101" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5">
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-    </row>
-    <row r="103" spans="2:5">
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-    </row>
-    <row r="104" spans="2:5">
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-    </row>
-    <row r="105" spans="2:5">
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-    </row>
-    <row r="106" spans="2:5">
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-    </row>
-    <row r="107" ht="23.25" customHeight="1" spans="1:1">
-      <c r="A107" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B108" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B109" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5">
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-    </row>
-    <row r="111" spans="2:5">
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-    </row>
-    <row r="112" spans="2:5">
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-    </row>
-    <row r="113" spans="2:5">
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="2:5">
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="26">
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="B4:C4"/>
@@ -2374,53 +1667,12 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="A27:E27"/>
-    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="F35:J35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="F43:J43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="F51:J51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="F59:J59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="A99:E99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
     <mergeCell ref="A1:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2435,7 +1687,7 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2448,7 +1700,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2474,10 +1726,10 @@
     </row>
     <row r="3" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
@@ -2494,9 +1746,9 @@
         <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
       <c r="B5" s="4" t="s">
@@ -2523,12 +1775,12 @@
       <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" customFormat="1" spans="2:10">
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" customFormat="1" spans="2:11">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2538,6 +1790,9 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
+      <c r="K6" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="1" spans="2:10">
       <c r="B7" s="5"/>
@@ -2585,10 +1840,10 @@
     </row>
     <row r="11" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -2688,10 +1943,10 @@
     </row>
     <row r="19" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -2791,10 +2046,10 @@
     </row>
     <row r="27" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -2894,10 +2149,10 @@
     </row>
     <row r="35" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -2997,10 +2252,10 @@
     </row>
     <row r="43" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -3100,10 +2355,10 @@
     </row>
     <row r="51" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -3203,10 +2458,10 @@
     </row>
     <row r="59" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
@@ -3306,7 +2561,7 @@
     </row>
     <row r="67" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A67" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3363,7 +2618,7 @@
     </row>
     <row r="75" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A75" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3420,7 +2675,7 @@
     </row>
     <row r="83" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A83" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3477,7 +2732,7 @@
     </row>
     <row r="91" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A91" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3534,7 +2789,7 @@
     </row>
     <row r="99" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A99" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3591,7 +2846,7 @@
     </row>
     <row r="107" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A107" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
@@ -3725,14 +2980,1295 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:N114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="3.875" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="8.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" spans="2:14">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="2:11">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A51" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" ht="23.25" customHeight="1" spans="1:6">
+      <c r="A59" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" spans="2:9">
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A67" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B68" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A75" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A83" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B84" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+    </row>
+    <row r="88" spans="2:5">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" spans="2:5">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+    </row>
+    <row r="91" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A91" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B92" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+    </row>
+    <row r="96" spans="2:5">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+    </row>
+    <row r="97" spans="2:5">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+    </row>
+    <row r="98" spans="2:5">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+    </row>
+    <row r="99" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A99" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B100" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+    </row>
+    <row r="103" spans="2:5">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+    </row>
+    <row r="104" spans="2:5">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+    </row>
+    <row r="106" spans="2:5">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+    </row>
+    <row r="107" ht="23.25" customHeight="1" spans="1:1">
+      <c r="A107" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B108" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="2:5">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+    </row>
+    <row r="114" spans="2:5">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="67">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="F35:J35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="F51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="F59:J59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A1:J2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1. prepare for wan to wifi iperf throughput
</commit_message>
<xml_diff>
--- a/throughput.xlsx
+++ b/throughput.xlsx
@@ -8,23 +8,24 @@
   </bookViews>
   <sheets>
     <sheet name="WAN" sheetId="1" r:id="rId1"/>
-    <sheet name="LAN" sheetId="2" r:id="rId2"/>
-    <sheet name="DUT" sheetId="3" r:id="rId3"/>
+    <sheet name="DUT" sheetId="2" r:id="rId2"/>
+    <sheet name="LAN" sheetId="3" r:id="rId3"/>
+    <sheet name="SPEEDTEST" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>WAN 2 WiFi/WiFi 2 WAN</t>
   </si>
   <si>
-    <t>CH11</t>
+    <t>CH36 20M</t>
   </si>
   <si>
-    <t>CH149</t>
+    <t>CH1 20M</t>
   </si>
   <si>
     <t xml:space="preserve">Downlink(Mbps)  </t>
@@ -33,40 +34,13 @@
     <t xml:space="preserve">Uplink(Mbps) </t>
   </si>
   <si>
-    <t>Throughput on this page is generated by Ookla speedtest</t>
+    <t>Throughput on this page is generated by iperf2</t>
   </si>
   <si>
     <t>PSK2</t>
   </si>
   <si>
     <t>CLEAR</t>
-  </si>
-  <si>
-    <t>CH11 WRELAY</t>
-  </si>
-  <si>
-    <t>CH149 WRELAY</t>
-  </si>
-  <si>
-    <t>CH11 RELAY</t>
-  </si>
-  <si>
-    <t>CH149 RELAY</t>
-  </si>
-  <si>
-    <t>GUEST</t>
-  </si>
-  <si>
-    <t>LAN 2 WiFi/WiFi 2 LAN</t>
-  </si>
-  <si>
-    <t>CH36 20M</t>
-  </si>
-  <si>
-    <t>CH1 20M</t>
-  </si>
-  <si>
-    <t>Throughput on this page is generated by iperf2</t>
   </si>
   <si>
     <t>BREAK means iperf stream break off</t>
@@ -137,18 +111,48 @@
   <si>
     <t>DUT 2 WiFi/WiFi 2 DUT</t>
   </si>
+  <si>
+    <t>LAN 2 WiFi/WiFi 2 LAN</t>
+  </si>
+  <si>
+    <t>OOKLA SPEEDTEST</t>
+  </si>
+  <si>
+    <t>CH11</t>
+  </si>
+  <si>
+    <t>CH149</t>
+  </si>
+  <si>
+    <t>Throughput on this page is generated by Ookla speedtest</t>
+  </si>
+  <si>
+    <t>CH11 WRELAY</t>
+  </si>
+  <si>
+    <t>CH149 WRELAY</t>
+  </si>
+  <si>
+    <t>CH11 RELAY</t>
+  </si>
+  <si>
+    <t>CH149 RELAY</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +198,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -201,39 +226,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,6 +266,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -278,7 +280,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,32 +316,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,10 +332,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -366,7 +377,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,6 +444,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,19 +521,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,48 +561,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -557,30 +568,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -595,6 +582,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,11 +619,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,170 +668,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,8 +832,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1167,20 +1180,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="6" max="6" width="2.875" customWidth="1"/>
-    <col min="11" max="11" width="3.125" customWidth="1"/>
+    <col min="1" max="1" width="3.875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="9" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="10" customWidth="1"/>
+    <col min="4" max="5" width="9" style="10"/>
+    <col min="6" max="6" width="3.875" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" s="10" customFormat="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1210,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" s="10" customFormat="1" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1206,32 +1222,45 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" ht="23.25" spans="1:6">
+    <row r="3" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" spans="2:11">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E4" s="3"/>
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" spans="2:10">
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1256,8 +1285,12 @@
       <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:10">
+      <c r="K5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" s="10" customFormat="1" spans="2:11">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1267,8 +1300,11 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:10">
+      <c r="K6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" s="10" customFormat="1" spans="2:10">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1279,7 +1315,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" s="10" customFormat="1" spans="2:10">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1290,7 +1326,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" s="10" customFormat="1" spans="2:10">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1301,7 +1337,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" s="10" customFormat="1" spans="2:10">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1312,29 +1348,41 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" ht="23.25" spans="1:6">
+    <row r="11" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" spans="2:9">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E12" s="3"/>
       <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" ht="15.75" spans="2:10">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" s="10" customFormat="1" spans="2:10">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1371,7 +1419,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" s="10" customFormat="1" spans="2:10">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1382,7 +1430,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" s="10" customFormat="1" spans="2:10">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1393,7 +1441,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" s="10" customFormat="1" spans="2:10">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1404,7 +1452,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" s="10" customFormat="1" spans="2:10">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1415,29 +1463,41 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" ht="23.25" spans="1:6">
+    <row r="19" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="2:9">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E20" s="3"/>
       <c r="G20" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" spans="2:10">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1463,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" s="10" customFormat="1" spans="2:10">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1474,7 +1534,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" s="10" customFormat="1" spans="2:10">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1485,7 +1545,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" s="10" customFormat="1" spans="2:10">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1496,7 +1556,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" s="10" customFormat="1" spans="2:10">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1507,7 +1567,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" s="10" customFormat="1" spans="2:10">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1518,26 +1578,41 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" ht="23.25" spans="1:9">
+    <row r="27" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" ht="15.75" spans="2:10">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" ht="15.75" spans="2:10">
+      <c r="E28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1550,13 +1625,20 @@
       <c r="E29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="2:10">
+      <c r="G29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" s="10" customFormat="1" spans="2:10">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1567,7 +1649,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" s="10" customFormat="1" spans="2:10">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1578,7 +1660,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" s="10" customFormat="1" spans="2:10">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1589,7 +1671,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" s="10" customFormat="1" spans="2:10">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1600,54 +1682,857 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" s="10" customFormat="1" spans="2:10">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-    </row>
-    <row r="35" ht="15.75" spans="2:4">
-      <c r="B35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" ht="15.75" spans="2:5">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="2:5">
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
+      <c r="A35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" s="10" customFormat="1" spans="2:10">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="2:5">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" s="10" customFormat="1" spans="2:10">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="2:5">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" s="10" customFormat="1" spans="2:10">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="2:5">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" s="10" customFormat="1" spans="2:10">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" s="10" customFormat="1" spans="2:10">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" s="10" customFormat="1" spans="2:10">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" s="10" customFormat="1" spans="2:10">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" s="10" customFormat="1" spans="2:10">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" s="10" customFormat="1" spans="2:10">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" s="10" customFormat="1" spans="2:10">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
+      <c r="A51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" s="10" customFormat="1" spans="2:10">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" s="10" customFormat="1" spans="2:10">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" s="10" customFormat="1" spans="2:10">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" s="10" customFormat="1" spans="2:10">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" s="10" customFormat="1" spans="2:10">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:10">
+      <c r="A59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="G60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+      <c r="B61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" s="10" customFormat="1" spans="2:10">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" s="10" customFormat="1" spans="2:10">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" s="10" customFormat="1" spans="2:10">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" s="10" customFormat="1" spans="2:10">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" s="10" customFormat="1" spans="2:10">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B68" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" s="10" customFormat="1" spans="2:5">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" s="10" customFormat="1" spans="2:5">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" s="10" customFormat="1" spans="2:5">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" s="10" customFormat="1" spans="2:5">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" s="10" customFormat="1" spans="2:5">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A75" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" s="10" customFormat="1" spans="2:5">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" s="10" customFormat="1" spans="2:5">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" s="10" customFormat="1" spans="2:5">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" s="10" customFormat="1" spans="2:5">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" s="10" customFormat="1" spans="2:5">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A83" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B84" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" s="10" customFormat="1" spans="2:5">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" s="10" customFormat="1" spans="2:5">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+    </row>
+    <row r="88" s="10" customFormat="1" spans="2:5">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" s="10" customFormat="1" spans="2:5">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" s="10" customFormat="1" spans="2:5">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+    </row>
+    <row r="91" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B92" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" s="10" customFormat="1" spans="2:5">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+    </row>
+    <row r="95" s="10" customFormat="1" spans="2:5">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+    </row>
+    <row r="96" s="10" customFormat="1" spans="2:5">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+    </row>
+    <row r="97" s="10" customFormat="1" spans="2:5">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+    </row>
+    <row r="98" s="10" customFormat="1" spans="2:5">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+    </row>
+    <row r="99" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B100" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" s="10" customFormat="1" spans="2:5">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+    </row>
+    <row r="103" s="10" customFormat="1" spans="2:5">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+    </row>
+    <row r="104" s="10" customFormat="1" spans="2:5">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+    </row>
+    <row r="105" s="10" customFormat="1" spans="2:5">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+    </row>
+    <row r="106" s="10" customFormat="1" spans="2:5">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+    </row>
+    <row r="107" s="10" customFormat="1" ht="23.25" customHeight="1" spans="1:5">
+      <c r="A107" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B108" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" s="10" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+      <c r="B109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" s="10" customFormat="1" spans="2:5">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" s="10" customFormat="1" spans="2:5">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" s="10" customFormat="1" spans="2:5">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" s="10" customFormat="1" spans="2:5">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+    </row>
+    <row r="114" s="10" customFormat="1" spans="2:5">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="67">
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="B4:C4"/>
@@ -1667,12 +2552,53 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="A27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="F27:J27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="F35:J35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="F51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="F59:J59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
     <mergeCell ref="A1:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1684,10 +2610,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:N114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1696,11 +2622,13 @@
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="8.875" customWidth="1"/>
     <col min="6" max="6" width="3.875" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:10">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1712,7 +2640,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" customFormat="1" spans="1:10">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1724,15 +2652,15 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="3" ht="23.25" customHeight="1" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" spans="2:14">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1746,11 +2674,12 @@
         <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
+        <v>5</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="2:11">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1776,11 +2705,10 @@
         <v>7</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" customFormat="1" spans="2:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1791,10 +2719,10 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="1" spans="2:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1805,7 +2733,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" customFormat="1" spans="2:10">
+    <row r="8" spans="2:10">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1816,7 +2744,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" customFormat="1" spans="2:10">
+    <row r="9" spans="2:10">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1827,7 +2755,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" customFormat="1" spans="2:10">
+    <row r="10" spans="2:10">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1838,15 +2766,15 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="11" ht="23.25" customHeight="1" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1860,7 +2788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="13" ht="15.75" customHeight="1" spans="2:10">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1886,7 +2814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="2:10">
+    <row r="14" spans="2:10">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1897,7 +2825,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" customFormat="1" spans="2:10">
+    <row r="15" spans="2:10">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1908,7 +2836,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" customFormat="1" spans="2:10">
+    <row r="16" spans="2:10">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1919,7 +2847,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" customFormat="1" spans="2:10">
+    <row r="17" spans="2:10">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1930,7 +2858,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" customFormat="1" spans="2:10">
+    <row r="18" spans="2:10">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1941,15 +2869,15 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="19" ht="23.25" customHeight="1" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" spans="2:9">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -1963,7 +2891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="21" ht="15.75" customHeight="1" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" customFormat="1" spans="2:10">
+    <row r="22" spans="2:10">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2000,7 +2928,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" customFormat="1" spans="2:10">
+    <row r="23" spans="2:10">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2011,7 +2939,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" customFormat="1" spans="2:10">
+    <row r="24" spans="2:10">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2022,7 +2950,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" customFormat="1" spans="2:10">
+    <row r="25" spans="2:10">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -2033,7 +2961,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" customFormat="1" spans="2:10">
+    <row r="26" spans="2:10">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -2044,15 +2972,15 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="27" ht="23.25" customHeight="1" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" spans="2:9">
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
@@ -2066,7 +2994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="29" ht="15.75" customHeight="1" spans="2:10">
       <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
@@ -2092,7 +3020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" customFormat="1" spans="2:10">
+    <row r="30" spans="2:10">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -2103,7 +3031,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" customFormat="1" spans="2:10">
+    <row r="31" spans="2:10">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2114,7 +3042,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" customFormat="1" spans="2:10">
+    <row r="32" spans="2:10">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -2125,7 +3053,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" customFormat="1" spans="2:10">
+    <row r="33" spans="2:10">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2136,7 +3064,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" customFormat="1" spans="2:10">
+    <row r="34" spans="2:10">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2147,15 +3075,15 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="35" ht="23.25" customHeight="1" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" spans="2:9">
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
@@ -2169,7 +3097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="37" ht="15.75" customHeight="1" spans="2:10">
       <c r="B37" s="4" t="s">
         <v>6</v>
       </c>
@@ -2195,7 +3123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="1" spans="2:10">
+    <row r="38" spans="2:10">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -2206,7 +3134,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" customFormat="1" spans="2:10">
+    <row r="39" spans="2:10">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -2217,7 +3145,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" customFormat="1" spans="2:10">
+    <row r="40" spans="2:10">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -2228,7 +3156,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" customFormat="1" spans="2:10">
+    <row r="41" spans="2:10">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2239,7 +3167,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" customFormat="1" spans="2:10">
+    <row r="42" spans="2:10">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -2250,15 +3178,15 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="43" ht="23.25" customHeight="1" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" spans="2:9">
       <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
@@ -2272,7 +3200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="45" ht="15.75" customHeight="1" spans="2:10">
       <c r="B45" s="4" t="s">
         <v>6</v>
       </c>
@@ -2298,7 +3226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" customFormat="1" spans="2:10">
+    <row r="46" spans="2:10">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2309,7 +3237,7 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" customFormat="1" spans="2:10">
+    <row r="47" spans="2:10">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2320,7 +3248,7 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" customFormat="1" spans="2:10">
+    <row r="48" spans="2:10">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -2331,7 +3259,7 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" customFormat="1" spans="2:10">
+    <row r="49" spans="2:10">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -2342,7 +3270,7 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" customFormat="1" spans="2:10">
+    <row r="50" spans="2:10">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2353,15 +3281,15 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="51" ht="23.25" customHeight="1" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1" spans="2:9">
       <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
@@ -2375,7 +3303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="53" ht="15.75" customHeight="1" spans="2:10">
       <c r="B53" s="4" t="s">
         <v>6</v>
       </c>
@@ -2401,7 +3329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" customFormat="1" spans="2:10">
+    <row r="54" spans="2:10">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2412,7 +3340,7 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" customFormat="1" spans="2:10">
+    <row r="55" spans="2:10">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2423,7 +3351,7 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" customFormat="1" spans="2:10">
+    <row r="56" spans="2:10">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2434,7 +3362,7 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" customFormat="1" spans="2:10">
+    <row r="57" spans="2:10">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -2445,7 +3373,7 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" customFormat="1" spans="2:10">
+    <row r="58" spans="2:10">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -2456,15 +3384,15 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
+    <row r="59" ht="23.25" customHeight="1" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" spans="2:9">
       <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
@@ -2478,7 +3406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
+    <row r="61" ht="15.75" customHeight="1" spans="2:10">
       <c r="B61" s="4" t="s">
         <v>6</v>
       </c>
@@ -2504,7 +3432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" customFormat="1" spans="2:10">
+    <row r="62" spans="2:10">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -2515,7 +3443,7 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" customFormat="1" spans="2:10">
+    <row r="63" spans="2:10">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -2526,7 +3454,7 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" customFormat="1" spans="2:10">
+    <row r="64" spans="2:10">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -2537,7 +3465,7 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" customFormat="1" spans="2:10">
+    <row r="65" spans="2:10">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2548,7 +3476,7 @@
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" customFormat="1" spans="2:10">
+    <row r="66" spans="2:10">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2559,12 +3487,12 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="67" ht="23.25" customHeight="1" spans="1:1">
       <c r="A67" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1" spans="2:4">
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
@@ -2572,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="69" ht="15.75" customHeight="1" spans="2:5">
       <c r="B69" s="4" t="s">
         <v>6</v>
       </c>
@@ -2586,42 +3514,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" customFormat="1" spans="2:5">
+    <row r="70" spans="2:5">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" customFormat="1" spans="2:5">
+    <row r="71" spans="2:5">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" customFormat="1" spans="2:5">
+    <row r="72" spans="2:5">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" customFormat="1" spans="2:5">
+    <row r="73" spans="2:5">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
-    <row r="74" customFormat="1" spans="2:5">
+    <row r="74" spans="2:5">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
-    <row r="75" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="75" ht="23.25" customHeight="1" spans="1:1">
       <c r="A75" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75" customHeight="1" spans="2:4">
       <c r="B76" s="3" t="s">
         <v>3</v>
       </c>
@@ -2629,7 +3557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="77" ht="15.75" customHeight="1" spans="2:5">
       <c r="B77" s="4" t="s">
         <v>6</v>
       </c>
@@ -2643,42 +3571,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" customFormat="1" spans="2:5">
+    <row r="78" spans="2:5">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" customFormat="1" spans="2:5">
+    <row r="79" spans="2:5">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" customFormat="1" spans="2:5">
+    <row r="80" spans="2:5">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" customFormat="1" spans="2:5">
+    <row r="81" spans="2:5">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" customFormat="1" spans="2:5">
+    <row r="82" spans="2:5">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="83" ht="23.25" customHeight="1" spans="1:1">
       <c r="A83" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" ht="15.75" customHeight="1" spans="2:4">
       <c r="B84" s="3" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +3614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="85" ht="15.75" customHeight="1" spans="2:5">
       <c r="B85" s="4" t="s">
         <v>6</v>
       </c>
@@ -2700,42 +3628,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" customFormat="1" spans="2:5">
+    <row r="86" spans="2:5">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
     </row>
-    <row r="87" customFormat="1" spans="2:5">
+    <row r="87" spans="2:5">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
     </row>
-    <row r="88" customFormat="1" spans="2:5">
+    <row r="88" spans="2:5">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
     </row>
-    <row r="89" customFormat="1" spans="2:5">
+    <row r="89" spans="2:5">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
     </row>
-    <row r="90" customFormat="1" spans="2:5">
+    <row r="90" spans="2:5">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
     </row>
-    <row r="91" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="91" ht="23.25" customHeight="1" spans="1:1">
       <c r="A91" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="92" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" ht="15.75" customHeight="1" spans="2:4">
       <c r="B92" s="3" t="s">
         <v>3</v>
       </c>
@@ -2743,7 +3671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="93" ht="15.75" customHeight="1" spans="2:5">
       <c r="B93" s="4" t="s">
         <v>6</v>
       </c>
@@ -2757,42 +3685,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" customFormat="1" spans="2:5">
+    <row r="94" spans="2:5">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
     </row>
-    <row r="95" customFormat="1" spans="2:5">
+    <row r="95" spans="2:5">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
     </row>
-    <row r="96" customFormat="1" spans="2:5">
+    <row r="96" spans="2:5">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
     </row>
-    <row r="97" customFormat="1" spans="2:5">
+    <row r="97" spans="2:5">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
     </row>
-    <row r="98" customFormat="1" spans="2:5">
+    <row r="98" spans="2:5">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
     </row>
-    <row r="99" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="99" ht="23.25" customHeight="1" spans="1:1">
       <c r="A99" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="100" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" ht="15.75" customHeight="1" spans="2:4">
       <c r="B100" s="3" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +3728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="101" ht="15.75" customHeight="1" spans="2:5">
       <c r="B101" s="4" t="s">
         <v>6</v>
       </c>
@@ -2814,42 +3742,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" customFormat="1" spans="2:5">
+    <row r="102" spans="2:5">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
     </row>
-    <row r="103" customFormat="1" spans="2:5">
+    <row r="103" spans="2:5">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
     </row>
-    <row r="104" customFormat="1" spans="2:5">
+    <row r="104" spans="2:5">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
     </row>
-    <row r="105" customFormat="1" spans="2:5">
+    <row r="105" spans="2:5">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
     </row>
-    <row r="106" customFormat="1" spans="2:5">
+    <row r="106" spans="2:5">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
     </row>
-    <row r="107" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
+    <row r="107" ht="23.25" customHeight="1" spans="1:1">
       <c r="A107" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="108" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1" spans="2:4">
       <c r="B108" s="3" t="s">
         <v>3</v>
       </c>
@@ -2857,7 +3785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
+    <row r="109" ht="15.75" customHeight="1" spans="2:5">
       <c r="B109" s="4" t="s">
         <v>6</v>
       </c>
@@ -2871,31 +3799,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" customFormat="1" spans="2:5">
+    <row r="110" spans="2:5">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
     </row>
-    <row r="111" customFormat="1" spans="2:5">
+    <row r="111" spans="2:5">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
     </row>
-    <row r="112" customFormat="1" spans="2:5">
+    <row r="112" spans="2:5">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
     </row>
-    <row r="113" customFormat="1" spans="2:5">
+    <row r="113" spans="2:5">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
     </row>
-    <row r="114" customFormat="1" spans="2:5">
+    <row r="114" spans="2:5">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -2980,10 +3908,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2992,13 +3920,11 @@
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="8.875" customWidth="1"/>
     <col min="6" max="6" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="9.125" customWidth="1"/>
-    <col min="12" max="12" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" customFormat="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3010,7 +3936,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" customFormat="1" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3022,15 +3948,15 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" ht="23.25" customHeight="1" spans="1:6">
+    <row r="3" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" spans="2:14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3044,12 +3970,11 @@
         <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" spans="2:11">
+        <v>5</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" customFormat="1" ht="15.75" customHeight="1" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3075,10 +4000,11 @@
         <v>7</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
+        <v>8</v>
+      </c>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" customFormat="1" spans="2:11">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3089,10 +4015,10 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="2:10">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3103,7 +4029,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" customFormat="1" spans="2:10">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3114,7 +4040,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" customFormat="1" spans="2:10">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3125,7 +4051,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" customFormat="1" spans="2:10">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3136,15 +4062,19 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" ht="23.25" customHeight="1" spans="1:6">
+    <row r="11" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" spans="2:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
@@ -3158,7 +4088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="2:10">
+    <row r="13" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -3184,7 +4114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" customFormat="1" spans="2:10">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3195,7 +4125,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" customFormat="1" spans="2:10">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3206,7 +4136,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" customFormat="1" spans="2:10">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3217,7 +4147,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" customFormat="1" spans="2:10">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3228,7 +4158,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" customFormat="1" spans="2:10">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3239,15 +4169,15 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" ht="23.25" customHeight="1" spans="1:6">
+    <row r="19" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1" spans="2:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -3261,7 +4191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="2:10">
+    <row r="21" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -3287,7 +4217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" customFormat="1" spans="2:10">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -3298,7 +4228,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" customFormat="1" spans="2:10">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3309,7 +4239,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" customFormat="1" spans="2:10">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3320,7 +4250,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" customFormat="1" spans="2:10">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3331,7 +4261,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" customFormat="1" spans="2:10">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -3342,15 +4272,15 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" ht="23.25" customHeight="1" spans="1:6">
+    <row r="27" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" spans="2:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
@@ -3364,7 +4294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1" spans="2:10">
+    <row r="29" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
@@ -3390,7 +4320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" customFormat="1" spans="2:10">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -3401,7 +4331,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" customFormat="1" spans="2:10">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -3412,7 +4342,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" customFormat="1" spans="2:10">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -3423,7 +4353,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" customFormat="1" spans="2:10">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -3434,7 +4364,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" customFormat="1" spans="2:10">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -3445,15 +4375,15 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" ht="23.25" customHeight="1" spans="1:6">
+    <row r="35" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" spans="2:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
@@ -3467,7 +4397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1" spans="2:10">
+    <row r="37" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B37" s="4" t="s">
         <v>6</v>
       </c>
@@ -3493,7 +4423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" customFormat="1" spans="2:10">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -3504,7 +4434,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" customFormat="1" spans="2:10">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -3515,7 +4445,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" customFormat="1" spans="2:10">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -3526,7 +4456,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="2:10">
+    <row r="41" customFormat="1" spans="2:10">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -3537,7 +4467,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" customFormat="1" spans="2:10">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -3548,15 +4478,15 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" ht="23.25" customHeight="1" spans="1:6">
+    <row r="43" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1" spans="2:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
@@ -3570,7 +4500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1" spans="2:10">
+    <row r="45" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B45" s="4" t="s">
         <v>6</v>
       </c>
@@ -3596,7 +4526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" customFormat="1" spans="2:10">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -3607,7 +4537,7 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" customFormat="1" spans="2:10">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -3618,7 +4548,7 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -3629,7 +4559,7 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" customFormat="1" spans="2:10">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -3640,7 +4570,7 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="2:10">
+    <row r="50" customFormat="1" spans="2:10">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -3651,15 +4581,15 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" ht="23.25" customHeight="1" spans="1:6">
+    <row r="51" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1" spans="2:9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
@@ -3673,7 +4603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1" spans="2:10">
+    <row r="53" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B53" s="4" t="s">
         <v>6</v>
       </c>
@@ -3699,7 +4629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:10">
+    <row r="54" customFormat="1" spans="2:10">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -3710,7 +4640,7 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="2:10">
+    <row r="55" customFormat="1" spans="2:10">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -3721,7 +4651,7 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" customFormat="1" spans="2:10">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -3732,7 +4662,7 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="2:10">
+    <row r="57" customFormat="1" spans="2:10">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -3743,7 +4673,7 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="2:10">
+    <row r="58" customFormat="1" spans="2:10">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -3754,15 +4684,15 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" ht="23.25" customHeight="1" spans="1:6">
+    <row r="59" customFormat="1" ht="23.25" customHeight="1" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1" spans="2:9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" customFormat="1" ht="15.75" customHeight="1" spans="2:9">
       <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
@@ -3776,7 +4706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1" spans="2:10">
+    <row r="61" customFormat="1" ht="15.75" customHeight="1" spans="2:10">
       <c r="B61" s="4" t="s">
         <v>6</v>
       </c>
@@ -3802,7 +4732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:10">
+    <row r="62" customFormat="1" spans="2:10">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -3813,7 +4743,7 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="2:10">
+    <row r="63" customFormat="1" spans="2:10">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -3824,7 +4754,7 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="2:10">
+    <row r="64" customFormat="1" spans="2:10">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -3835,7 +4765,7 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="2:10">
+    <row r="65" customFormat="1" spans="2:10">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -3846,7 +4776,7 @@
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10">
+    <row r="66" customFormat="1" spans="2:10">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -3857,12 +4787,12 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" ht="23.25" customHeight="1" spans="1:1">
+    <row r="67" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A67" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" ht="15.75" customHeight="1" spans="2:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
@@ -3870,7 +4800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1" spans="2:5">
+    <row r="69" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B69" s="4" t="s">
         <v>6</v>
       </c>
@@ -3884,42 +4814,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:5">
+    <row r="70" customFormat="1" spans="2:5">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="2:5">
+    <row r="71" customFormat="1" spans="2:5">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="2:5">
+    <row r="72" customFormat="1" spans="2:5">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="2:5">
+    <row r="73" customFormat="1" spans="2:5">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
-    <row r="74" spans="2:5">
+    <row r="74" customFormat="1" spans="2:5">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
-    <row r="75" ht="23.25" customHeight="1" spans="1:1">
+    <row r="75" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A75" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" ht="15.75" customHeight="1" spans="2:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B76" s="3" t="s">
         <v>3</v>
       </c>
@@ -3927,7 +4857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1" spans="2:5">
+    <row r="77" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B77" s="4" t="s">
         <v>6</v>
       </c>
@@ -3941,42 +4871,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:5">
+    <row r="78" customFormat="1" spans="2:5">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="2:5">
+    <row r="79" customFormat="1" spans="2:5">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="2:5">
+    <row r="80" customFormat="1" spans="2:5">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" customFormat="1" spans="2:5">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" customFormat="1" spans="2:5">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" ht="23.25" customHeight="1" spans="1:1">
+    <row r="83" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A83" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" ht="15.75" customHeight="1" spans="2:4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B84" s="3" t="s">
         <v>3</v>
       </c>
@@ -3984,7 +4914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" ht="15.75" customHeight="1" spans="2:5">
+    <row r="85" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B85" s="4" t="s">
         <v>6</v>
       </c>
@@ -3998,42 +4928,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="2:5">
+    <row r="86" customFormat="1" spans="2:5">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
     </row>
-    <row r="87" spans="2:5">
+    <row r="87" customFormat="1" spans="2:5">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
     </row>
-    <row r="88" spans="2:5">
+    <row r="88" customFormat="1" spans="2:5">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
     </row>
-    <row r="89" spans="2:5">
+    <row r="89" customFormat="1" spans="2:5">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
     </row>
-    <row r="90" spans="2:5">
+    <row r="90" customFormat="1" spans="2:5">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
     </row>
-    <row r="91" ht="23.25" customHeight="1" spans="1:1">
+    <row r="91" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A91" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="92" ht="15.75" customHeight="1" spans="2:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B92" s="3" t="s">
         <v>3</v>
       </c>
@@ -4041,7 +4971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" ht="15.75" customHeight="1" spans="2:5">
+    <row r="93" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B93" s="4" t="s">
         <v>6</v>
       </c>
@@ -4055,42 +4985,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="2:5">
+    <row r="94" customFormat="1" spans="2:5">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
     </row>
-    <row r="95" spans="2:5">
+    <row r="95" customFormat="1" spans="2:5">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
     </row>
-    <row r="96" spans="2:5">
+    <row r="96" customFormat="1" spans="2:5">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
     </row>
-    <row r="97" spans="2:5">
+    <row r="97" customFormat="1" spans="2:5">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
     </row>
-    <row r="98" spans="2:5">
+    <row r="98" customFormat="1" spans="2:5">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
     </row>
-    <row r="99" ht="23.25" customHeight="1" spans="1:1">
+    <row r="99" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A99" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="100" ht="15.75" customHeight="1" spans="2:4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B100" s="3" t="s">
         <v>3</v>
       </c>
@@ -4098,7 +5028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" ht="15.75" customHeight="1" spans="2:5">
+    <row r="101" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B101" s="4" t="s">
         <v>6</v>
       </c>
@@ -4112,42 +5042,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="2:5">
+    <row r="102" customFormat="1" spans="2:5">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
     </row>
-    <row r="103" spans="2:5">
+    <row r="103" customFormat="1" spans="2:5">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
     </row>
-    <row r="104" spans="2:5">
+    <row r="104" customFormat="1" spans="2:5">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
     </row>
-    <row r="105" spans="2:5">
+    <row r="105" customFormat="1" spans="2:5">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
     </row>
-    <row r="106" spans="2:5">
+    <row r="106" customFormat="1" spans="2:5">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
     </row>
-    <row r="107" ht="23.25" customHeight="1" spans="1:1">
+    <row r="107" customFormat="1" ht="23.25" customHeight="1" spans="1:1">
       <c r="A107" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1" spans="2:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" customFormat="1" ht="15.75" customHeight="1" spans="2:4">
       <c r="B108" s="3" t="s">
         <v>3</v>
       </c>
@@ -4155,7 +5085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" ht="15.75" customHeight="1" spans="2:5">
+    <row r="109" customFormat="1" ht="15.75" customHeight="1" spans="2:5">
       <c r="B109" s="4" t="s">
         <v>6</v>
       </c>
@@ -4169,31 +5099,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="2:5">
+    <row r="110" customFormat="1" spans="2:5">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
     </row>
-    <row r="111" spans="2:5">
+    <row r="111" customFormat="1" spans="2:5">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
     </row>
-    <row r="112" spans="2:5">
+    <row r="112" customFormat="1" spans="2:5">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
     </row>
-    <row r="113" spans="2:5">
+    <row r="113" customFormat="1" spans="2:5">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
     </row>
-    <row r="114" spans="2:5">
+    <row r="114" customFormat="1" spans="2:5">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4273,4 +5203,521 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:K41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="6" max="6" width="2.875" customWidth="1"/>
+    <col min="11" max="11" width="3.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" ht="23.25" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="2:11">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="2:10">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" ht="23.25" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="2:9">
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="2:10">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" ht="23.25" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" spans="2:9">
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" spans="2:10">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" ht="23.25" spans="1:9">
+      <c r="A27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" ht="15.75" spans="2:10">
+      <c r="B28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" ht="15.75" spans="2:10">
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" ht="15.75" spans="2:4">
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" ht="15.75" spans="2:5">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="A1:J2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>